<commit_message>
nueva logica para elegir:grupo a y b
</commit_message>
<xml_diff>
--- a/laliga/realmadrid/realmadrid.xlsx
+++ b/laliga/realmadrid/realmadrid.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomip\OneDrive\Documentos\pucelale\pucelale.local\laliga\realmadrid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAEF9E8-192F-4E0E-92DE-83C07E9B9BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6E7A78-9329-4570-8A55-C37CF3A0977E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{71052352-51EA-43E8-AFE1-BD72E05A4F60}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71052352-51EA-43E8-AFE1-BD72E05A4F60}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -500,10 +500,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,11 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D86A48B-8925-49D5-A679-578BAA46DFEC}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,7 +870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -892,7 +890,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -912,7 +910,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -932,7 +930,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -952,7 +950,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -992,7 +990,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1012,7 +1010,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -1032,7 +1030,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1072,7 +1070,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1112,7 +1110,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1132,7 +1130,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1152,7 +1150,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1172,7 +1170,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1192,7 +1190,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1212,7 +1210,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1252,7 +1250,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1272,7 +1270,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1292,7 +1290,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1312,7 +1310,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1332,7 +1330,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1352,7 +1350,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1372,7 +1370,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1412,7 +1410,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1432,7 +1430,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -1452,7 +1450,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1472,7 +1470,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1492,7 +1490,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1512,7 +1510,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -1532,7 +1530,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -1552,7 +1550,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -1572,7 +1570,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -1592,7 +1590,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -1612,7 +1610,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -1632,7 +1630,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -1672,7 +1670,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -1712,7 +1710,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -1732,7 +1730,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -1752,7 +1750,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -1772,7 +1770,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -1792,7 +1790,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -1812,7 +1810,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -1832,7 +1830,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -1852,7 +1850,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -1872,7 +1870,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -1912,7 +1910,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>83</v>
       </c>
@@ -1932,7 +1930,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -1952,7 +1950,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -1972,7 +1970,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1992,7 +1990,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -2012,7 +2010,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -2052,7 +2050,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -2072,7 +2070,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -2092,7 +2090,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>94</v>
       </c>
@@ -2112,7 +2110,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>93</v>
       </c>
@@ -2132,7 +2130,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>97</v>
       </c>
@@ -2152,7 +2150,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>90</v>
       </c>
@@ -2192,7 +2190,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>101</v>
       </c>
@@ -2212,7 +2210,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>102</v>
       </c>
@@ -2232,7 +2230,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>98</v>
       </c>
@@ -2252,7 +2250,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>96</v>
       </c>
@@ -2292,7 +2290,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -2312,7 +2310,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>120</v>
       </c>
@@ -2332,7 +2330,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -2352,7 +2350,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -2372,7 +2370,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>57</v>
       </c>
@@ -2392,7 +2390,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>110</v>
       </c>
@@ -2412,7 +2410,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -2432,7 +2430,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>109</v>
       </c>
@@ -2452,7 +2450,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>117</v>
       </c>
@@ -2492,7 +2490,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>108</v>
       </c>
@@ -2552,7 +2550,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>124</v>
       </c>
@@ -2572,7 +2570,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -2592,7 +2590,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>125</v>
       </c>
@@ -2672,7 +2670,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>131</v>
       </c>
@@ -2685,7 +2683,7 @@
       <c r="D92">
         <v>29</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92">
         <v>2023</v>
       </c>
       <c r="F92">
@@ -2712,7 +2710,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>134</v>
       </c>
@@ -2873,12 +2871,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F96" xr:uid="{2D86A48B-8925-49D5-A679-578BAA46DFEC}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="2025"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:F101" xr:uid="{2D86A48B-8925-49D5-A679-578BAA46DFEC}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:F100">
       <sortCondition ref="D1:D96"/>
     </sortState>

</xml_diff>